<commit_message>
i may have been too mean the first time around
</commit_message>
<xml_diff>
--- a/changes/m4-handguards.xlsx
+++ b/changes/m4-handguards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lingl\Documents\deadline-balancing\changes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACB66D7C-72FB-4ADD-B463-4552F3EAD783}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C46BD41-369F-4406-BE44-0E3B7547641E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="124">
   <si>
     <t>new</t>
   </si>
@@ -366,6 +366,45 @@
   </si>
   <si>
     <t>KAC URX 6 MLOK 13"</t>
+  </si>
+  <si>
+    <t>mk10_bottom_adapter_large</t>
+  </si>
+  <si>
+    <t>MK10RL Large</t>
+  </si>
+  <si>
+    <t>mk10_bottom_adapter_small</t>
+  </si>
+  <si>
+    <t>MK10RL Small</t>
+  </si>
+  <si>
+    <t>mk10_side_adapter_large</t>
+  </si>
+  <si>
+    <t>mk10_side_adapter_small</t>
+  </si>
+  <si>
+    <t>mk10_top_adapter_large</t>
+  </si>
+  <si>
+    <t>fab_defense_upr_16_4_bottom</t>
+  </si>
+  <si>
+    <t>FAB Defense UPR 16/4 Picatinny Rail</t>
+  </si>
+  <si>
+    <t>ncstar_marsv2_bottom</t>
+  </si>
+  <si>
+    <t>NcStar MARSV2 Picatinny Rail</t>
+  </si>
+  <si>
+    <t>fab_defense_upr_16_4_top</t>
+  </si>
+  <si>
+    <t>ncstar_marsv2_top</t>
   </si>
 </sst>
 </file>
@@ -1207,14 +1246,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N50"/>
+  <dimension ref="A1:N61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q17" sqref="Q17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="13.7109375" customWidth="1"/>
     <col min="2" max="2" width="49" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1306,7 +1346,7 @@
         <v>0</v>
       </c>
       <c r="N3" s="1">
-        <f>C3-D3*20-E3*0.8-F3*0.6-H3*5+I3*10+J3/300</f>
+        <f t="shared" ref="N3:N11" si="0">C3-D3*20-E3*0.8-F3*0.6-H3*5+I3*10+J3/300</f>
         <v>23.75</v>
       </c>
     </row>
@@ -1327,7 +1367,7 @@
         <v>-11</v>
       </c>
       <c r="F4">
-        <v>-17</v>
+        <v>-16</v>
       </c>
       <c r="H4">
         <v>0.08</v>
@@ -1336,8 +1376,8 @@
         <v>500</v>
       </c>
       <c r="N4" s="1">
-        <f>C4-D4*20-E4*0.8-F4*0.6-H4*5+I4*10+J4/300</f>
-        <v>24.8</v>
+        <f t="shared" si="0"/>
+        <v>24.200000000000003</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -1357,7 +1397,7 @@
         <v>-10</v>
       </c>
       <c r="F5">
-        <v>-16</v>
+        <v>-15</v>
       </c>
       <c r="H5">
         <v>7.0000000000000007E-2</v>
@@ -1366,8 +1406,8 @@
         <v>600</v>
       </c>
       <c r="N5" s="1">
-        <f>C5-D5*20-E5*0.8-F5*0.6-H5*5+I5*10+J5/300</f>
-        <v>24.849999999999998</v>
+        <f t="shared" si="0"/>
+        <v>24.25</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -1381,10 +1421,10 @@
         <v>11</v>
       </c>
       <c r="D6">
-        <v>0.3</v>
+        <v>0.32</v>
       </c>
       <c r="E6">
-        <v>-11</v>
+        <v>-10</v>
       </c>
       <c r="F6">
         <v>-18</v>
@@ -1393,8 +1433,8 @@
         <v>900</v>
       </c>
       <c r="N6" s="1">
-        <f>C6-D6*20-E6*0.8-F6*0.6-H6*5+I6*10+J6/300</f>
-        <v>24.6</v>
+        <f t="shared" si="0"/>
+        <v>23.4</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -1408,10 +1448,10 @@
         <v>9</v>
       </c>
       <c r="D7">
-        <v>0.34</v>
+        <v>0.36</v>
       </c>
       <c r="E7">
-        <v>-13</v>
+        <v>-12</v>
       </c>
       <c r="F7">
         <v>-20</v>
@@ -1420,8 +1460,8 @@
         <v>950</v>
       </c>
       <c r="N7" s="1">
-        <f>C7-D7*20-E7*0.8-F7*0.6-H7*5+I7*10+J7/300</f>
-        <v>24.6</v>
+        <f t="shared" si="0"/>
+        <v>23.400000000000002</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -1447,7 +1487,7 @@
         <v>1000</v>
       </c>
       <c r="N8" s="1">
-        <f>C8-D8*20-E8*0.8-F8*0.6-H8*5+I8*10+J8/300</f>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
     </row>
@@ -1474,7 +1514,7 @@
         <v>1000</v>
       </c>
       <c r="N9" s="1">
-        <f>C9-D9*20-E9*0.8-F9*0.6-H9*5+I9*10+J9/300</f>
+        <f t="shared" si="0"/>
         <v>19.200000000000003</v>
       </c>
     </row>
@@ -1501,7 +1541,7 @@
         <v>1000</v>
       </c>
       <c r="N10" s="1">
-        <f>C10-D10*20-E10*0.8-F10*0.6-H10*5+I10*10+J10/300</f>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
     </row>
@@ -1528,7 +1568,7 @@
         <v>1100</v>
       </c>
       <c r="N11" s="1">
-        <f>C11-D11*20-E11*0.8-F11*0.6-H11*5+I11*10+J11/300</f>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
     </row>
@@ -1555,7 +1595,7 @@
         <v>1100</v>
       </c>
       <c r="N12" s="1">
-        <f t="shared" ref="N12:N50" si="0">C12-D12*20-E12*0.8-F12*0.6-H12*5+I12*10+J12/300</f>
+        <f t="shared" ref="N12:N61" si="1">C12-D12*20-E12*0.8-F12*0.6-H12*5+I12*10+J12/300</f>
         <v>18.8</v>
       </c>
     </row>
@@ -1585,7 +1625,7 @@
         <v>700</v>
       </c>
       <c r="N13" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>17.8</v>
       </c>
     </row>
@@ -1612,7 +1652,7 @@
         <v>0</v>
       </c>
       <c r="N14" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1642,7 +1682,7 @@
         <v>1200</v>
       </c>
       <c r="N15" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>19.400000000000002</v>
       </c>
     </row>
@@ -1669,7 +1709,7 @@
         <v>950</v>
       </c>
       <c r="N16" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>18.399999999999999</v>
       </c>
     </row>
@@ -1696,7 +1736,7 @@
         <v>900</v>
       </c>
       <c r="N17" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>18.599999999999998</v>
       </c>
     </row>
@@ -1723,7 +1763,7 @@
         <v>750</v>
       </c>
       <c r="N18" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
     </row>
@@ -1771,14 +1811,14 @@
         <v>-4</v>
       </c>
       <c r="F20">
-        <v>-7</v>
+        <v>-8</v>
       </c>
       <c r="M20">
         <v>500</v>
       </c>
       <c r="N20" s="1">
         <f>C20-D20*20-E20*0.8-F20*0.6-H20*5+I20*10+J20/300</f>
-        <v>17.2</v>
+        <v>17.8</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
@@ -1798,14 +1838,14 @@
         <v>-6</v>
       </c>
       <c r="F21">
-        <v>-9</v>
+        <v>-10</v>
       </c>
       <c r="M21">
         <v>550</v>
       </c>
       <c r="N21" s="1">
         <f>C21-D21*20-E21*0.8-F21*0.6-H21*5+I21*10+J21/300</f>
-        <v>17.2</v>
+        <v>17.8</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
@@ -1831,7 +1871,7 @@
         <v>600</v>
       </c>
       <c r="N22" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>17.399999999999999</v>
       </c>
     </row>
@@ -1858,7 +1898,7 @@
         <v>800</v>
       </c>
       <c r="N23" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>17.399999999999999</v>
       </c>
     </row>
@@ -1885,7 +1925,7 @@
         <v>1000</v>
       </c>
       <c r="N24" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>18.399999999999999</v>
       </c>
     </row>
@@ -1912,7 +1952,7 @@
         <v>1200</v>
       </c>
       <c r="N25" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
     </row>
@@ -1939,7 +1979,7 @@
         <v>950</v>
       </c>
       <c r="N26" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>18.2</v>
       </c>
     </row>
@@ -1966,7 +2006,7 @@
         <v>900</v>
       </c>
       <c r="N27" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>18.2</v>
       </c>
     </row>
@@ -1984,17 +2024,17 @@
         <v>0.24</v>
       </c>
       <c r="E28">
-        <v>-4</v>
+        <v>-5</v>
       </c>
       <c r="F28">
-        <v>-10</v>
+        <v>-9</v>
       </c>
       <c r="M28">
         <v>800</v>
       </c>
       <c r="N28" s="1">
-        <f t="shared" si="0"/>
-        <v>18.399999999999999</v>
+        <f t="shared" si="1"/>
+        <v>18.599999999999998</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
@@ -2020,7 +2060,7 @@
         <v>1500</v>
       </c>
       <c r="N29" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>20.2</v>
       </c>
     </row>
@@ -2038,124 +2078,124 @@
         <v>0.24</v>
       </c>
       <c r="E30">
-        <v>-9</v>
+        <v>-8</v>
       </c>
       <c r="F30">
-        <v>-8</v>
+        <v>-10</v>
       </c>
       <c r="M30">
         <v>1100</v>
       </c>
       <c r="N30" s="1">
-        <f t="shared" si="0"/>
-        <v>19.2</v>
+        <f t="shared" si="1"/>
+        <v>19.600000000000001</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>21</v>
+      </c>
+      <c r="B31" t="s">
+        <v>22</v>
+      </c>
+      <c r="C31">
         <v>15</v>
       </c>
-      <c r="B31" t="s">
-        <v>16</v>
-      </c>
-      <c r="C31">
-        <v>13</v>
-      </c>
       <c r="D31">
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
       <c r="E31">
-        <v>-8</v>
+        <v>-6</v>
       </c>
       <c r="F31">
-        <v>-7</v>
+        <v>-5</v>
       </c>
       <c r="M31">
-        <v>750</v>
+        <v>700</v>
       </c>
       <c r="N31" s="1">
         <f>C31-D31*20-E31*0.8-F31*0.6-H31*5+I31*10+J31/300</f>
-        <v>18.600000000000001</v>
+        <v>18.8</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B32" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C32">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D32">
-        <v>0.28000000000000003</v>
+        <v>0.25</v>
       </c>
       <c r="E32">
-        <v>-10</v>
+        <v>-8</v>
       </c>
       <c r="F32">
-        <v>-8</v>
+        <v>-7</v>
       </c>
       <c r="M32">
-        <v>800</v>
+        <v>750</v>
       </c>
       <c r="N32" s="1">
-        <f>C32-D32*20-E32*0.8-F32*0.6-H32*5+I32*10+J32/300</f>
-        <v>18.2</v>
+        <f t="shared" ref="N32:N39" si="2">C32-D32*20-E32*0.8-F32*0.6-H32*5+I32*10+J32/300</f>
+        <v>18.600000000000001</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B33" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C33">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D33">
-        <v>0.33</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="E33">
-        <v>-12</v>
+        <v>-10</v>
       </c>
       <c r="F33">
-        <v>-10</v>
+        <v>-9</v>
       </c>
       <c r="M33">
-        <v>900</v>
+        <v>800</v>
       </c>
       <c r="N33" s="1">
-        <f>C33-D33*20-E33*0.8-F33*0.6-H33*5+I33*10+J33/300</f>
-        <v>18</v>
+        <f t="shared" si="2"/>
+        <v>18.799999999999997</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B34" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C34">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D34">
-        <v>0.2</v>
+        <v>0.33</v>
       </c>
       <c r="E34">
-        <v>-5</v>
+        <v>-12</v>
       </c>
       <c r="F34">
-        <v>-6</v>
+        <v>-11</v>
       </c>
       <c r="M34">
-        <v>700</v>
+        <v>900</v>
       </c>
       <c r="N34" s="1">
-        <f>C34-D34*20-E34*0.8-F34*0.6-H34*5+I34*10+J34/300</f>
+        <f t="shared" si="2"/>
         <v>18.600000000000001</v>
       </c>
     </row>
@@ -2182,7 +2222,7 @@
         <v>1100</v>
       </c>
       <c r="N35" s="1">
-        <f>C35-D35*20-E35*0.8-F35*0.6-H35*5+I35*10+J35/300</f>
+        <f t="shared" si="2"/>
         <v>19.400000000000002</v>
       </c>
     </row>
@@ -2203,14 +2243,14 @@
         <v>-11</v>
       </c>
       <c r="F36">
-        <v>-7</v>
+        <v>-8</v>
       </c>
       <c r="M36">
         <v>1000</v>
       </c>
       <c r="N36" s="1">
-        <f>C36-D36*20-E36*0.8-F36*0.6-H36*5+I36*10+J36/300</f>
-        <v>18.8</v>
+        <f t="shared" si="2"/>
+        <v>19.400000000000002</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
@@ -2230,14 +2270,14 @@
         <v>-12</v>
       </c>
       <c r="F37">
-        <v>-8</v>
+        <v>-9</v>
       </c>
       <c r="M37">
         <v>1050</v>
       </c>
       <c r="N37" s="1">
-        <f>C37-D37*20-E37*0.8-F37*0.6-H37*5+I37*10+J37/300</f>
-        <v>18.600000000000001</v>
+        <f t="shared" si="2"/>
+        <v>19.2</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
@@ -2257,14 +2297,14 @@
         <v>-13</v>
       </c>
       <c r="F38">
-        <v>-11</v>
+        <v>-12</v>
       </c>
       <c r="M38">
         <v>1100</v>
       </c>
       <c r="N38" s="1">
-        <f>C38-D38*20-E38*0.8-F38*0.6-H38*5+I38*10+J38/300</f>
-        <v>18.399999999999999</v>
+        <f t="shared" si="2"/>
+        <v>19</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
@@ -2281,7 +2321,7 @@
         <v>0.36</v>
       </c>
       <c r="E39">
-        <v>-14</v>
+        <v>-15</v>
       </c>
       <c r="F39">
         <v>-12</v>
@@ -2290,8 +2330,8 @@
         <v>1200</v>
       </c>
       <c r="N39" s="1">
-        <f>C39-D39*20-E39*0.8-F39*0.6-H39*5+I39*10+J39/300</f>
-        <v>18.200000000000003</v>
+        <f t="shared" si="2"/>
+        <v>19</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
@@ -2317,7 +2357,7 @@
         <v>1500</v>
       </c>
       <c r="N40" s="1">
-        <f t="shared" ref="N40:N41" si="1">C40-D40*20-E40*0.8-F40*0.6-H40*5+I40*10+J40/300</f>
+        <f t="shared" ref="N40:N41" si="3">C40-D40*20-E40*0.8-F40*0.6-H40*5+I40*10+J40/300</f>
         <v>19.399999999999999</v>
       </c>
     </row>
@@ -2344,7 +2384,7 @@
         <v>1100</v>
       </c>
       <c r="N41" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>19.2</v>
       </c>
     </row>
@@ -2446,14 +2486,14 @@
         <v>-5</v>
       </c>
       <c r="F45">
-        <v>-11</v>
+        <v>-10</v>
       </c>
       <c r="M45">
         <v>1300</v>
       </c>
       <c r="N45" s="1">
-        <f t="shared" si="0"/>
-        <v>19.799999999999997</v>
+        <f t="shared" si="1"/>
+        <v>19.2</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
@@ -2473,14 +2513,14 @@
         <v>-6</v>
       </c>
       <c r="F46">
-        <v>-14</v>
+        <v>-13</v>
       </c>
       <c r="M46">
         <v>1350</v>
       </c>
       <c r="N46" s="1">
-        <f t="shared" si="0"/>
-        <v>19.8</v>
+        <f t="shared" si="1"/>
+        <v>19.2</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
@@ -2506,7 +2546,7 @@
         <v>1400</v>
       </c>
       <c r="N47" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>19.600000000000001</v>
       </c>
     </row>
@@ -2533,7 +2573,7 @@
         <v>1450</v>
       </c>
       <c r="N48" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>19.599999999999998</v>
       </c>
     </row>
@@ -2560,7 +2600,7 @@
         <v>1500</v>
       </c>
       <c r="N49" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
     </row>
@@ -2581,14 +2621,239 @@
         <v>-12</v>
       </c>
       <c r="F50">
-        <v>-19</v>
+        <v>-20</v>
       </c>
       <c r="M50">
         <v>1600</v>
       </c>
       <c r="N50" s="1">
-        <f t="shared" si="0"/>
-        <v>17.600000000000001</v>
+        <f t="shared" si="1"/>
+        <v>18.200000000000003</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N51" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>111</v>
+      </c>
+      <c r="B52" t="s">
+        <v>112</v>
+      </c>
+      <c r="C52">
+        <v>-1</v>
+      </c>
+      <c r="D52">
+        <v>0.1</v>
+      </c>
+      <c r="E52">
+        <v>2</v>
+      </c>
+      <c r="F52">
+        <v>2</v>
+      </c>
+      <c r="M52">
+        <v>0</v>
+      </c>
+      <c r="N52" s="1">
+        <f t="shared" si="1"/>
+        <v>-5.8</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>113</v>
+      </c>
+      <c r="B53" t="s">
+        <v>114</v>
+      </c>
+      <c r="C53">
+        <v>-1</v>
+      </c>
+      <c r="D53">
+        <v>0.04</v>
+      </c>
+      <c r="E53">
+        <v>2</v>
+      </c>
+      <c r="F53">
+        <v>2</v>
+      </c>
+      <c r="M53">
+        <v>0</v>
+      </c>
+      <c r="N53" s="1">
+        <f t="shared" si="1"/>
+        <v>-4.6000000000000005</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>115</v>
+      </c>
+      <c r="B54" t="s">
+        <v>112</v>
+      </c>
+      <c r="C54">
+        <v>-1</v>
+      </c>
+      <c r="D54">
+        <v>0.1</v>
+      </c>
+      <c r="M54">
+        <v>0</v>
+      </c>
+      <c r="N54" s="1">
+        <f t="shared" si="1"/>
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>116</v>
+      </c>
+      <c r="B55" t="s">
+        <v>114</v>
+      </c>
+      <c r="C55">
+        <v>-1</v>
+      </c>
+      <c r="D55">
+        <v>0.04</v>
+      </c>
+      <c r="M55">
+        <v>0</v>
+      </c>
+      <c r="N55" s="1">
+        <f t="shared" si="1"/>
+        <v>-1.8</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>117</v>
+      </c>
+      <c r="B56" t="s">
+        <v>112</v>
+      </c>
+      <c r="C56">
+        <v>-1</v>
+      </c>
+      <c r="D56">
+        <v>0.1</v>
+      </c>
+      <c r="M56">
+        <v>0</v>
+      </c>
+      <c r="N56" s="1">
+        <f t="shared" si="1"/>
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N57" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>118</v>
+      </c>
+      <c r="B58" t="s">
+        <v>119</v>
+      </c>
+      <c r="C58">
+        <v>-3</v>
+      </c>
+      <c r="D58">
+        <v>0.06</v>
+      </c>
+      <c r="E58">
+        <v>2</v>
+      </c>
+      <c r="F58">
+        <v>2</v>
+      </c>
+      <c r="M58">
+        <v>400</v>
+      </c>
+      <c r="N58" s="1">
+        <f t="shared" si="1"/>
+        <v>-7.0000000000000009</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>120</v>
+      </c>
+      <c r="B59" t="s">
+        <v>121</v>
+      </c>
+      <c r="C59">
+        <v>-2</v>
+      </c>
+      <c r="D59">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E59">
+        <v>1</v>
+      </c>
+      <c r="F59">
+        <v>5</v>
+      </c>
+      <c r="M59">
+        <v>300</v>
+      </c>
+      <c r="N59" s="1">
+        <f t="shared" si="1"/>
+        <v>-7.2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>122</v>
+      </c>
+      <c r="B60" t="s">
+        <v>119</v>
+      </c>
+      <c r="C60">
+        <v>-3</v>
+      </c>
+      <c r="D60">
+        <v>0.06</v>
+      </c>
+      <c r="M60">
+        <v>400</v>
+      </c>
+      <c r="N60" s="1">
+        <f t="shared" si="1"/>
+        <v>-4.2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>123</v>
+      </c>
+      <c r="B61" t="s">
+        <v>121</v>
+      </c>
+      <c r="C61">
+        <v>-2</v>
+      </c>
+      <c r="D61">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="M61">
+        <v>300</v>
+      </c>
+      <c r="N61" s="1">
+        <f t="shared" si="1"/>
+        <v>-3.4000000000000004</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
kac and warsport handguards
</commit_message>
<xml_diff>
--- a/changes/m4-handguards.xlsx
+++ b/changes/m4-handguards.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lingl\Documents\deadline-balancing\changes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yifan\Documents\deadline-balancing\changes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74563F78-3EA1-4C4D-BB91-79A3F5C18EAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0395FC14-15BE-4E5C-B40F-989149B2FF77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="m4-barrels" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="138">
   <si>
     <t>new</t>
   </si>
@@ -176,36 +176,9 @@
     <t>KAC M5 RAS Upper Handguard</t>
   </si>
   <si>
-    <t>kac_mre_ras_free_float_12inch</t>
-  </si>
-  <si>
     <t xml:space="preserve">KAC MRE RAS Free Float 12" </t>
   </si>
   <si>
-    <t>kac_ras_free_float_12inch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KAC RAS Free Float 12" </t>
-  </si>
-  <si>
-    <t>kac_ras_free_float_5inch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KAC RAS Free Float 5" </t>
-  </si>
-  <si>
-    <t>lvoa_c_handguard</t>
-  </si>
-  <si>
-    <t>LVOA-C</t>
-  </si>
-  <si>
-    <t>lvoa_s_handguard</t>
-  </si>
-  <si>
-    <t>LVOA-S</t>
-  </si>
-  <si>
     <t>monster_10i_type_a_handguard</t>
   </si>
   <si>
@@ -411,6 +384,69 @@
   </si>
   <si>
     <t>Colt 607 CAR-15 Triangle 7" Handguard</t>
+  </si>
+  <si>
+    <t>kac_mre_free_float_ras_rifle_12inch_handguard</t>
+  </si>
+  <si>
+    <t>kac_free_float_ras_medium_long_10.375inch_handguard</t>
+  </si>
+  <si>
+    <t>KAC Free Float RAS Medium Long 10.375"</t>
+  </si>
+  <si>
+    <t>kac_mre_standard_front_filler_tube</t>
+  </si>
+  <si>
+    <t>KAC MRE Standard Front Filler Tube</t>
+  </si>
+  <si>
+    <t>kac_mre_railed_front_filler_tube</t>
+  </si>
+  <si>
+    <t>KAC MRE Railed Front Filler Tube</t>
+  </si>
+  <si>
+    <t>kac_free_float_ras_rifle_12inch_handguard</t>
+  </si>
+  <si>
+    <t>kac_free_float_ras_carbine_7inch_handguard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KAC Free Float RAS Carbine 7" </t>
+  </si>
+  <si>
+    <t xml:space="preserve">KAC Free Float RAS Rifle 12" </t>
+  </si>
+  <si>
+    <t>warsport_lvoa_s_13.5inch_handguard</t>
+  </si>
+  <si>
+    <t>warsport_lvoa_c_16.25inch_handguard</t>
+  </si>
+  <si>
+    <t>Warsport LVOA-S 13.5" Handguard</t>
+  </si>
+  <si>
+    <t>Warsport LVOA-C 16.25" Handguard</t>
+  </si>
+  <si>
+    <t>warsport_handguard_long_accessory_rail_bottom</t>
+  </si>
+  <si>
+    <t>warsport_handguard_long_accessory_rail_side</t>
+  </si>
+  <si>
+    <t>warsport_handguard_short_accessory_rail_bottom</t>
+  </si>
+  <si>
+    <t>warsport_handguard_short_accessory_rail_side</t>
+  </si>
+  <si>
+    <t>Warsport Long Accessory Rail</t>
+  </si>
+  <si>
+    <t>Warsport Short Accessory Rail</t>
   </si>
 </sst>
 </file>
@@ -1252,10 +1288,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N62"/>
+  <dimension ref="A1:N70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="P18" sqref="P18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1328,10 +1364,10 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="B3" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="C3">
         <v>14</v>
@@ -1352,16 +1388,16 @@
         <v>0</v>
       </c>
       <c r="N3" s="1">
-        <f t="shared" ref="N3:N12" si="0">C3-D3*20-E3*0.8-F3*0.6-H3*5+I3*10+J3/300</f>
+        <f t="shared" ref="N3:N23" si="0">C3-D3*20-E3*0.8-F3*0.6-H3*5+I3*10+J3/300</f>
         <v>23.75</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="B4" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="C4">
         <v>12</v>
@@ -1418,10 +1454,10 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="B6" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="C6">
         <v>16</v>
@@ -1448,64 +1484,64 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>53</v>
+        <v>128</v>
       </c>
       <c r="B7" t="s">
-        <v>54</v>
+        <v>130</v>
       </c>
       <c r="C7">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D7">
         <v>0.32</v>
       </c>
       <c r="E7">
-        <v>-10</v>
+        <v>-9</v>
       </c>
       <c r="F7">
-        <v>-18</v>
+        <v>-14</v>
       </c>
       <c r="M7">
         <v>900</v>
       </c>
       <c r="N7" s="1">
         <f t="shared" si="0"/>
-        <v>23.4</v>
+        <v>18.200000000000003</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>55</v>
+        <v>129</v>
       </c>
       <c r="B8" t="s">
-        <v>56</v>
+        <v>131</v>
       </c>
       <c r="C8">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D8">
         <v>0.36</v>
       </c>
       <c r="E8">
-        <v>-12</v>
+        <v>-11</v>
       </c>
       <c r="F8">
-        <v>-20</v>
+        <v>-16</v>
       </c>
       <c r="M8">
         <v>950</v>
       </c>
       <c r="N8" s="1">
         <f t="shared" si="0"/>
-        <v>23.400000000000002</v>
+        <v>18.200000000000003</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="B9" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C9">
         <v>13</v>
@@ -1631,7 +1667,7 @@
         <v>1100</v>
       </c>
       <c r="N13" s="1">
-        <f t="shared" ref="N13:N62" si="1">C13-D13*20-E13*0.8-F13*0.6-H13*5+I13*10+J13/300</f>
+        <f t="shared" si="0"/>
         <v>18.8</v>
       </c>
     </row>
@@ -1661,7 +1697,7 @@
         <v>700</v>
       </c>
       <c r="N14" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>17.8</v>
       </c>
     </row>
@@ -1672,23 +1708,11 @@
       <c r="B15" t="s">
         <v>44</v>
       </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
       <c r="M15">
         <v>0</v>
       </c>
       <c r="N15" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1706,10 +1730,10 @@
         <v>0.34</v>
       </c>
       <c r="E16">
-        <v>-11</v>
+        <v>-13</v>
       </c>
       <c r="F16">
-        <v>-16</v>
+        <v>-13</v>
       </c>
       <c r="H16">
         <v>0.04</v>
@@ -1718,1178 +1742,1340 @@
         <v>1200</v>
       </c>
       <c r="N16" s="1">
-        <f t="shared" si="1"/>
-        <v>19.400000000000002</v>
+        <f t="shared" si="0"/>
+        <v>19.2</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>117</v>
+      </c>
+      <c r="B17" t="s">
         <v>47</v>
-      </c>
-      <c r="B17" t="s">
-        <v>48</v>
       </c>
       <c r="C17">
         <v>7</v>
       </c>
       <c r="D17">
-        <v>0.31</v>
+        <v>0.27</v>
       </c>
       <c r="E17">
+        <v>-11</v>
+      </c>
+      <c r="F17">
+        <v>-14</v>
+      </c>
+      <c r="M17">
+        <v>1400</v>
+      </c>
+      <c r="N17" s="1">
+        <f t="shared" si="0"/>
+        <v>18.8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>120</v>
+      </c>
+      <c r="B18" t="s">
+        <v>121</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>0.06</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18" s="1">
+        <f t="shared" si="0"/>
+        <v>-0.19999999999999996</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>122</v>
+      </c>
+      <c r="B19" t="s">
+        <v>123</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>0.1</v>
+      </c>
+      <c r="F19">
+        <v>-1</v>
+      </c>
+      <c r="M19">
+        <v>500</v>
+      </c>
+      <c r="N19" s="1">
+        <f t="shared" si="0"/>
+        <v>-0.4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>124</v>
+      </c>
+      <c r="B20" t="s">
+        <v>127</v>
+      </c>
+      <c r="C20">
+        <v>7</v>
+      </c>
+      <c r="D20">
+        <v>0.33</v>
+      </c>
+      <c r="E20">
         <v>-10</v>
       </c>
-      <c r="F17">
-        <v>-16</v>
-      </c>
-      <c r="M17">
-        <v>950</v>
-      </c>
-      <c r="N17" s="1">
+      <c r="F20">
+        <v>-17</v>
+      </c>
+      <c r="M20">
+        <v>900</v>
+      </c>
+      <c r="N20" s="1">
+        <f t="shared" si="0"/>
+        <v>18.599999999999998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>118</v>
+      </c>
+      <c r="B21" t="s">
+        <v>119</v>
+      </c>
+      <c r="C21">
+        <v>9</v>
+      </c>
+      <c r="D21">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="E21">
+        <v>-8</v>
+      </c>
+      <c r="F21">
+        <v>-15</v>
+      </c>
+      <c r="M21">
+        <v>1200</v>
+      </c>
+      <c r="N21" s="1">
+        <f t="shared" si="0"/>
+        <v>18.8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>125</v>
+      </c>
+      <c r="B22" t="s">
+        <v>126</v>
+      </c>
+      <c r="C22">
+        <v>11</v>
+      </c>
+      <c r="D22">
+        <v>0.21</v>
+      </c>
+      <c r="E22">
+        <v>-5</v>
+      </c>
+      <c r="F22">
+        <v>-12</v>
+      </c>
+      <c r="M22">
+        <v>750</v>
+      </c>
+      <c r="N22" s="1">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23">
+        <v>14</v>
+      </c>
+      <c r="D23">
+        <v>0.13</v>
+      </c>
+      <c r="E23">
+        <v>-2</v>
+      </c>
+      <c r="F23">
+        <v>-5</v>
+      </c>
+      <c r="M23">
+        <v>700</v>
+      </c>
+      <c r="N23" s="1">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>56</v>
+      </c>
+      <c r="B24" t="s">
+        <v>57</v>
+      </c>
+      <c r="C24">
+        <v>14</v>
+      </c>
+      <c r="D24">
+        <v>0.21</v>
+      </c>
+      <c r="E24">
+        <v>-4</v>
+      </c>
+      <c r="F24">
+        <v>-8</v>
+      </c>
+      <c r="M24">
+        <v>500</v>
+      </c>
+      <c r="N24" s="1">
+        <f>C24-D24*20-E24*0.8-F24*0.6-H24*5+I24*10+J24/300</f>
+        <v>17.8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>58</v>
+      </c>
+      <c r="B25" t="s">
+        <v>59</v>
+      </c>
+      <c r="C25">
+        <v>12</v>
+      </c>
+      <c r="D25">
+        <v>0.25</v>
+      </c>
+      <c r="E25">
+        <v>-6</v>
+      </c>
+      <c r="F25">
+        <v>-10</v>
+      </c>
+      <c r="M25">
+        <v>550</v>
+      </c>
+      <c r="N25" s="1">
+        <f>C25-D25*20-E25*0.8-F25*0.6-H25*5+I25*10+J25/300</f>
+        <v>17.8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>48</v>
+      </c>
+      <c r="B26" t="s">
+        <v>49</v>
+      </c>
+      <c r="C26">
+        <v>8</v>
+      </c>
+      <c r="D26">
+        <v>0.27</v>
+      </c>
+      <c r="E26">
+        <v>-8</v>
+      </c>
+      <c r="F26">
+        <v>-14</v>
+      </c>
+      <c r="M26">
+        <v>600</v>
+      </c>
+      <c r="N26" s="1">
+        <f t="shared" ref="N26:N70" si="1">C26-D26*20-E26*0.8-F26*0.6-H26*5+I26*10+J26/300</f>
+        <v>17.399999999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27">
+        <v>6</v>
+      </c>
+      <c r="D27">
+        <v>0.34</v>
+      </c>
+      <c r="E27">
+        <v>-10</v>
+      </c>
+      <c r="F27">
+        <v>-17</v>
+      </c>
+      <c r="M27">
+        <v>800</v>
+      </c>
+      <c r="N27" s="1">
+        <f t="shared" si="1"/>
+        <v>17.399999999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>60</v>
+      </c>
+      <c r="B28" t="s">
+        <v>61</v>
+      </c>
+      <c r="C28">
+        <v>9</v>
+      </c>
+      <c r="D28">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="E28">
+        <v>-10</v>
+      </c>
+      <c r="F28">
+        <v>-12</v>
+      </c>
+      <c r="M28">
+        <v>1000</v>
+      </c>
+      <c r="N28" s="1">
         <f t="shared" si="1"/>
         <v>18.399999999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>49</v>
-      </c>
-      <c r="B18" t="s">
-        <v>50</v>
-      </c>
-      <c r="C18">
-        <v>7</v>
-      </c>
-      <c r="D18">
-        <v>0.33</v>
-      </c>
-      <c r="E18">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>62</v>
+      </c>
+      <c r="B29" t="s">
+        <v>63</v>
+      </c>
+      <c r="C29">
+        <v>6</v>
+      </c>
+      <c r="D29">
+        <v>0.36</v>
+      </c>
+      <c r="E29">
+        <v>-12</v>
+      </c>
+      <c r="F29">
+        <v>-16</v>
+      </c>
+      <c r="M29">
+        <v>1200</v>
+      </c>
+      <c r="N29" s="1">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>64</v>
+      </c>
+      <c r="B30" t="s">
+        <v>65</v>
+      </c>
+      <c r="C30">
+        <v>11</v>
+      </c>
+      <c r="D30">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="E30">
+        <v>-7</v>
+      </c>
+      <c r="F30">
+        <v>-12</v>
+      </c>
+      <c r="M30">
+        <v>950</v>
+      </c>
+      <c r="N30" s="1">
+        <f t="shared" si="1"/>
+        <v>18.2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>66</v>
+      </c>
+      <c r="B31" t="s">
+        <v>67</v>
+      </c>
+      <c r="C31">
+        <v>8</v>
+      </c>
+      <c r="D31">
+        <v>0.34</v>
+      </c>
+      <c r="E31">
         <v>-10</v>
       </c>
-      <c r="F18">
-        <v>-17</v>
-      </c>
-      <c r="M18">
+      <c r="F31">
+        <v>-15</v>
+      </c>
+      <c r="M31">
         <v>900</v>
       </c>
-      <c r="N18" s="1">
+      <c r="N31" s="1">
+        <f t="shared" si="1"/>
+        <v>18.2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>82</v>
+      </c>
+      <c r="B32" t="s">
+        <v>83</v>
+      </c>
+      <c r="C32">
+        <v>14</v>
+      </c>
+      <c r="D32">
+        <v>0.24</v>
+      </c>
+      <c r="E32">
+        <v>-5</v>
+      </c>
+      <c r="F32">
+        <v>-9</v>
+      </c>
+      <c r="M32">
+        <v>800</v>
+      </c>
+      <c r="N32" s="1">
         <f t="shared" si="1"/>
         <v>18.599999999999998</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>51</v>
-      </c>
-      <c r="B19" t="s">
-        <v>52</v>
-      </c>
-      <c r="C19">
-        <v>11</v>
-      </c>
-      <c r="D19">
-        <v>0.21</v>
-      </c>
-      <c r="E19">
-        <v>-5</v>
-      </c>
-      <c r="F19">
-        <v>-12</v>
-      </c>
-      <c r="M19">
-        <v>750</v>
-      </c>
-      <c r="N19" s="1">
-        <f t="shared" si="1"/>
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>61</v>
-      </c>
-      <c r="B20" t="s">
-        <v>62</v>
-      </c>
-      <c r="C20">
-        <v>14</v>
-      </c>
-      <c r="D20">
-        <v>0.13</v>
-      </c>
-      <c r="E20">
-        <v>-2</v>
-      </c>
-      <c r="F20">
-        <v>-5</v>
-      </c>
-      <c r="M20">
-        <v>700</v>
-      </c>
-      <c r="N20" s="1">
-        <f>C20-D20*20-E20*0.8-F20*0.6-H20*5+I20*10+J20/300</f>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>65</v>
-      </c>
-      <c r="B21" t="s">
-        <v>66</v>
-      </c>
-      <c r="C21">
-        <v>14</v>
-      </c>
-      <c r="D21">
-        <v>0.21</v>
-      </c>
-      <c r="E21">
-        <v>-4</v>
-      </c>
-      <c r="F21">
-        <v>-8</v>
-      </c>
-      <c r="M21">
-        <v>500</v>
-      </c>
-      <c r="N21" s="1">
-        <f>C21-D21*20-E21*0.8-F21*0.6-H21*5+I21*10+J21/300</f>
-        <v>17.8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>67</v>
-      </c>
-      <c r="B22" t="s">
-        <v>68</v>
-      </c>
-      <c r="C22">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>84</v>
+      </c>
+      <c r="B33" t="s">
+        <v>85</v>
+      </c>
+      <c r="C33">
         <v>12</v>
       </c>
-      <c r="D22">
-        <v>0.25</v>
-      </c>
-      <c r="E22">
-        <v>-6</v>
-      </c>
-      <c r="F22">
-        <v>-10</v>
-      </c>
-      <c r="M22">
-        <v>550</v>
-      </c>
-      <c r="N22" s="1">
-        <f>C22-D22*20-E22*0.8-F22*0.6-H22*5+I22*10+J22/300</f>
-        <v>17.8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>57</v>
-      </c>
-      <c r="B23" t="s">
-        <v>58</v>
-      </c>
-      <c r="C23">
-        <v>8</v>
-      </c>
-      <c r="D23">
-        <v>0.27</v>
-      </c>
-      <c r="E23">
-        <v>-8</v>
-      </c>
-      <c r="F23">
-        <v>-14</v>
-      </c>
-      <c r="M23">
-        <v>600</v>
-      </c>
-      <c r="N23" s="1">
-        <f t="shared" si="1"/>
-        <v>17.399999999999999</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>59</v>
-      </c>
-      <c r="B24" t="s">
-        <v>60</v>
-      </c>
-      <c r="C24">
-        <v>6</v>
-      </c>
-      <c r="D24">
-        <v>0.34</v>
-      </c>
-      <c r="E24">
-        <v>-10</v>
-      </c>
-      <c r="F24">
-        <v>-17</v>
-      </c>
-      <c r="M24">
-        <v>800</v>
-      </c>
-      <c r="N24" s="1">
-        <f t="shared" si="1"/>
-        <v>17.399999999999999</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>69</v>
-      </c>
-      <c r="B25" t="s">
-        <v>70</v>
-      </c>
-      <c r="C25">
-        <v>9</v>
-      </c>
-      <c r="D25">
-        <v>0.28999999999999998</v>
-      </c>
-      <c r="E25">
-        <v>-10</v>
-      </c>
-      <c r="F25">
-        <v>-12</v>
-      </c>
-      <c r="M25">
-        <v>1000</v>
-      </c>
-      <c r="N25" s="1">
-        <f t="shared" si="1"/>
-        <v>18.399999999999999</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>71</v>
-      </c>
-      <c r="B26" t="s">
-        <v>72</v>
-      </c>
-      <c r="C26">
-        <v>6</v>
-      </c>
-      <c r="D26">
-        <v>0.36</v>
-      </c>
-      <c r="E26">
-        <v>-12</v>
-      </c>
-      <c r="F26">
-        <v>-16</v>
-      </c>
-      <c r="M26">
-        <v>1200</v>
-      </c>
-      <c r="N26" s="1">
-        <f t="shared" si="1"/>
-        <v>18</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>73</v>
-      </c>
-      <c r="B27" t="s">
-        <v>74</v>
-      </c>
-      <c r="C27">
-        <v>11</v>
-      </c>
-      <c r="D27">
+      <c r="D33">
         <v>0.28000000000000003</v>
       </c>
-      <c r="E27">
-        <v>-7</v>
-      </c>
-      <c r="F27">
-        <v>-12</v>
-      </c>
-      <c r="M27">
-        <v>950</v>
-      </c>
-      <c r="N27" s="1">
-        <f t="shared" si="1"/>
-        <v>18.2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>75</v>
-      </c>
-      <c r="B28" t="s">
-        <v>76</v>
-      </c>
-      <c r="C28">
-        <v>8</v>
-      </c>
-      <c r="D28">
-        <v>0.34</v>
-      </c>
-      <c r="E28">
-        <v>-10</v>
-      </c>
-      <c r="F28">
-        <v>-15</v>
-      </c>
-      <c r="M28">
-        <v>900</v>
-      </c>
-      <c r="N28" s="1">
-        <f t="shared" si="1"/>
-        <v>18.2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>91</v>
-      </c>
-      <c r="B29" t="s">
-        <v>92</v>
-      </c>
-      <c r="C29">
-        <v>14</v>
-      </c>
-      <c r="D29">
-        <v>0.24</v>
-      </c>
-      <c r="E29">
-        <v>-5</v>
-      </c>
-      <c r="F29">
+      <c r="E33">
         <v>-9</v>
       </c>
-      <c r="M29">
-        <v>800</v>
-      </c>
-      <c r="N29" s="1">
-        <f t="shared" si="1"/>
-        <v>18.599999999999998</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>93</v>
-      </c>
-      <c r="B30" t="s">
-        <v>94</v>
-      </c>
-      <c r="C30">
-        <v>12</v>
-      </c>
-      <c r="D30">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="E30">
-        <v>-9</v>
-      </c>
-      <c r="F30">
+      <c r="F33">
         <v>-11</v>
       </c>
-      <c r="M30">
+      <c r="M33">
         <v>1500</v>
       </c>
-      <c r="N30" s="1">
+      <c r="N33" s="1">
         <f t="shared" si="1"/>
         <v>20.2</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>95</v>
-      </c>
-      <c r="B31" t="s">
-        <v>96</v>
-      </c>
-      <c r="C31">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>86</v>
+      </c>
+      <c r="B34" t="s">
+        <v>87</v>
+      </c>
+      <c r="C34">
         <v>12</v>
       </c>
-      <c r="D31">
+      <c r="D34">
         <v>0.24</v>
       </c>
-      <c r="E31">
+      <c r="E34">
         <v>-8</v>
       </c>
-      <c r="F31">
+      <c r="F34">
         <v>-10</v>
       </c>
-      <c r="M31">
+      <c r="M34">
         <v>1100</v>
       </c>
-      <c r="N31" s="1">
+      <c r="N34" s="1">
         <f t="shared" si="1"/>
         <v>19.600000000000001</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>21</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B35" t="s">
         <v>22</v>
       </c>
-      <c r="C32">
+      <c r="C35">
         <v>15</v>
       </c>
-      <c r="D32">
+      <c r="D35">
         <v>0.2</v>
       </c>
-      <c r="E32">
+      <c r="E35">
         <v>-6</v>
       </c>
-      <c r="F32">
+      <c r="F35">
         <v>-5</v>
       </c>
-      <c r="M32">
+      <c r="M35">
         <v>700</v>
       </c>
-      <c r="N32" s="1">
-        <f>C32-D32*20-E32*0.8-F32*0.6-H32*5+I32*10+J32/300</f>
+      <c r="N35" s="1">
+        <f>C35-D35*20-E35*0.8-F35*0.6-H35*5+I35*10+J35/300</f>
         <v>18.8</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>15</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B36" t="s">
         <v>16</v>
       </c>
-      <c r="C33">
+      <c r="C36">
         <v>13</v>
       </c>
-      <c r="D33">
+      <c r="D36">
         <v>0.25</v>
       </c>
-      <c r="E33">
+      <c r="E36">
         <v>-8</v>
       </c>
-      <c r="F33">
+      <c r="F36">
         <v>-7</v>
       </c>
-      <c r="M33">
+      <c r="M36">
         <v>750</v>
       </c>
-      <c r="N33" s="1">
-        <f t="shared" ref="N33:N40" si="2">C33-D33*20-E33*0.8-F33*0.6-H33*5+I33*10+J33/300</f>
+      <c r="N36" s="1">
+        <f t="shared" ref="N36:N43" si="2">C36-D36*20-E36*0.8-F36*0.6-H36*5+I36*10+J36/300</f>
         <v>18.600000000000001</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>17</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B37" t="s">
         <v>18</v>
       </c>
-      <c r="C34">
+      <c r="C37">
         <v>11</v>
       </c>
-      <c r="D34">
+      <c r="D37">
         <v>0.28000000000000003</v>
       </c>
-      <c r="E34">
+      <c r="E37">
         <v>-10</v>
       </c>
-      <c r="F34">
+      <c r="F37">
         <v>-9</v>
       </c>
-      <c r="M34">
+      <c r="M37">
         <v>800</v>
       </c>
-      <c r="N34" s="1">
+      <c r="N37" s="1">
         <f t="shared" si="2"/>
         <v>18.799999999999997</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>19</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B38" t="s">
         <v>20</v>
       </c>
-      <c r="C35">
+      <c r="C38">
         <v>9</v>
       </c>
-      <c r="D35">
+      <c r="D38">
         <v>0.33</v>
       </c>
-      <c r="E35">
+      <c r="E38">
         <v>-12</v>
       </c>
-      <c r="F35">
+      <c r="F38">
         <v>-11</v>
       </c>
-      <c r="M35">
+      <c r="M38">
         <v>900</v>
       </c>
-      <c r="N35" s="1">
+      <c r="N38" s="1">
         <f t="shared" si="2"/>
         <v>18.600000000000001</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>81</v>
-      </c>
-      <c r="B36" t="s">
-        <v>82</v>
-      </c>
-      <c r="C36">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>72</v>
+      </c>
+      <c r="B39" t="s">
+        <v>73</v>
+      </c>
+      <c r="C39">
         <v>10</v>
       </c>
-      <c r="D36">
+      <c r="D39">
         <v>0.31</v>
       </c>
-      <c r="E36">
+      <c r="E39">
         <v>-12</v>
       </c>
-      <c r="F36">
+      <c r="F39">
         <v>-10</v>
       </c>
-      <c r="M36">
+      <c r="M39">
         <v>1100</v>
       </c>
-      <c r="N36" s="1">
+      <c r="N39" s="1">
         <f t="shared" si="2"/>
         <v>19.400000000000002</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>41</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B40" t="s">
         <v>42</v>
       </c>
-      <c r="C37">
+      <c r="C40">
         <v>11</v>
       </c>
-      <c r="D37">
+      <c r="D40">
         <v>0.26</v>
       </c>
-      <c r="E37">
+      <c r="E40">
         <v>-11</v>
       </c>
-      <c r="F37">
+      <c r="F40">
         <v>-8</v>
       </c>
-      <c r="M37">
+      <c r="M40">
         <v>1000</v>
       </c>
-      <c r="N37" s="1">
+      <c r="N40" s="1">
         <f t="shared" si="2"/>
         <v>19.400000000000002</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>79</v>
-      </c>
-      <c r="B38" t="s">
-        <v>80</v>
-      </c>
-      <c r="C38">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>70</v>
+      </c>
+      <c r="B41" t="s">
+        <v>71</v>
+      </c>
+      <c r="C41">
         <v>10</v>
       </c>
-      <c r="D38">
+      <c r="D41">
         <v>0.28999999999999998</v>
       </c>
-      <c r="E38">
+      <c r="E41">
         <v>-12</v>
       </c>
-      <c r="F38">
+      <c r="F41">
         <v>-9</v>
       </c>
-      <c r="M38">
+      <c r="M41">
         <v>1050</v>
       </c>
-      <c r="N38" s="1">
+      <c r="N41" s="1">
         <f t="shared" si="2"/>
         <v>19.2</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>37</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B42" t="s">
         <v>38</v>
       </c>
-      <c r="C39">
+      <c r="C42">
         <v>8</v>
       </c>
-      <c r="D39">
+      <c r="D42">
         <v>0.33</v>
       </c>
-      <c r="E39">
+      <c r="E42">
         <v>-13</v>
       </c>
-      <c r="F39">
+      <c r="F42">
         <v>-12</v>
       </c>
-      <c r="M39">
+      <c r="M42">
         <v>1100</v>
       </c>
-      <c r="N39" s="1">
+      <c r="N42" s="1">
         <f t="shared" si="2"/>
         <v>19</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>39</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B43" t="s">
         <v>40</v>
       </c>
-      <c r="C40">
+      <c r="C43">
         <v>7</v>
       </c>
-      <c r="D40">
+      <c r="D43">
         <v>0.36</v>
       </c>
-      <c r="E40">
+      <c r="E43">
         <v>-15</v>
       </c>
-      <c r="F40">
+      <c r="F43">
         <v>-12</v>
       </c>
-      <c r="M40">
+      <c r="M43">
         <v>1200</v>
       </c>
-      <c r="N40" s="1">
+      <c r="N43" s="1">
         <f t="shared" si="2"/>
         <v>19</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>109</v>
-      </c>
-      <c r="B41" t="s">
-        <v>110</v>
-      </c>
-      <c r="C41">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>100</v>
+      </c>
+      <c r="B44" t="s">
+        <v>101</v>
+      </c>
+      <c r="C44">
         <v>9</v>
       </c>
-      <c r="D41">
+      <c r="D44">
         <v>0.33</v>
       </c>
-      <c r="E41">
+      <c r="E44">
         <v>-10</v>
       </c>
-      <c r="F41">
+      <c r="F44">
         <v>-15</v>
       </c>
-      <c r="M41">
+      <c r="M44">
         <v>1500</v>
       </c>
-      <c r="N41" s="1">
-        <f t="shared" ref="N41:N42" si="3">C41-D41*20-E41*0.8-F41*0.6-H41*5+I41*10+J41/300</f>
+      <c r="N44" s="1">
+        <f t="shared" ref="N44:N45" si="3">C44-D44*20-E44*0.8-F44*0.6-H44*5+I44*10+J44/300</f>
         <v>19.399999999999999</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>83</v>
-      </c>
-      <c r="B42" t="s">
-        <v>84</v>
-      </c>
-      <c r="C42">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>74</v>
+      </c>
+      <c r="B45" t="s">
+        <v>75</v>
+      </c>
+      <c r="C45">
         <v>13</v>
       </c>
-      <c r="D42">
+      <c r="D45">
         <v>0.24</v>
       </c>
-      <c r="E42">
+      <c r="E45">
         <v>-7</v>
       </c>
-      <c r="F42">
+      <c r="F45">
         <v>-9</v>
       </c>
-      <c r="M42">
+      <c r="M45">
         <v>1100</v>
       </c>
-      <c r="N42" s="1">
+      <c r="N45" s="1">
         <f t="shared" si="3"/>
         <v>19.2</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>25</v>
-      </c>
-      <c r="B43" t="s">
-        <v>26</v>
-      </c>
-      <c r="C43">
-        <v>11</v>
-      </c>
-      <c r="D43">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="E43">
-        <v>-9</v>
-      </c>
-      <c r="F43">
-        <v>-11</v>
-      </c>
-      <c r="M43">
-        <v>1150</v>
-      </c>
-      <c r="N43" s="1">
-        <f>C43-D43*20-E43*0.8-F43*0.6-H43*5+I43*10+J43/300</f>
-        <v>19.2</v>
-      </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>85</v>
-      </c>
-      <c r="B44" t="s">
-        <v>86</v>
-      </c>
-      <c r="C44">
-        <v>9</v>
-      </c>
-      <c r="D44">
-        <v>0.32</v>
-      </c>
-      <c r="E44">
-        <v>-11</v>
-      </c>
-      <c r="F44">
-        <v>-13</v>
-      </c>
-      <c r="M44">
-        <v>1250</v>
-      </c>
-      <c r="N44" s="1">
-        <f>C44-D44*20-E44*0.8-F44*0.6-H44*5+I44*10+J44/300</f>
-        <v>19.2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>87</v>
-      </c>
-      <c r="B45" t="s">
-        <v>88</v>
-      </c>
-      <c r="C45">
-        <v>8</v>
-      </c>
-      <c r="D45">
-        <v>0.35</v>
-      </c>
-      <c r="E45">
-        <v>-12</v>
-      </c>
-      <c r="F45">
-        <v>-14</v>
-      </c>
-      <c r="M45">
-        <v>1300</v>
-      </c>
-      <c r="N45" s="1">
-        <f>C45-D45*20-E45*0.8-F45*0.6-H45*5+I45*10+J45/300</f>
-        <v>19</v>
-      </c>
-    </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>97</v>
+        <v>25</v>
       </c>
       <c r="B46" t="s">
-        <v>98</v>
+        <v>26</v>
       </c>
       <c r="C46">
+        <v>11</v>
+      </c>
+      <c r="D46">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="E46">
+        <v>-9</v>
+      </c>
+      <c r="F46">
+        <v>-11</v>
+      </c>
+      <c r="M46">
+        <v>1150</v>
+      </c>
+      <c r="N46" s="1">
+        <f>C46-D46*20-E46*0.8-F46*0.6-H46*5+I46*10+J46/300</f>
+        <v>19.2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>76</v>
+      </c>
+      <c r="B47" t="s">
+        <v>77</v>
+      </c>
+      <c r="C47">
+        <v>9</v>
+      </c>
+      <c r="D47">
+        <v>0.32</v>
+      </c>
+      <c r="E47">
+        <v>-11</v>
+      </c>
+      <c r="F47">
+        <v>-13</v>
+      </c>
+      <c r="M47">
+        <v>1250</v>
+      </c>
+      <c r="N47" s="1">
+        <f>C47-D47*20-E47*0.8-F47*0.6-H47*5+I47*10+J47/300</f>
+        <v>19.2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>78</v>
+      </c>
+      <c r="B48" t="s">
+        <v>79</v>
+      </c>
+      <c r="C48">
+        <v>8</v>
+      </c>
+      <c r="D48">
+        <v>0.35</v>
+      </c>
+      <c r="E48">
+        <v>-12</v>
+      </c>
+      <c r="F48">
+        <v>-14</v>
+      </c>
+      <c r="M48">
+        <v>1300</v>
+      </c>
+      <c r="N48" s="1">
+        <f>C48-D48*20-E48*0.8-F48*0.6-H48*5+I48*10+J48/300</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>88</v>
+      </c>
+      <c r="B49" t="s">
+        <v>89</v>
+      </c>
+      <c r="C49">
         <v>14</v>
       </c>
-      <c r="D46">
+      <c r="D49">
         <v>0.24</v>
       </c>
-      <c r="E46">
+      <c r="E49">
         <v>-5</v>
       </c>
-      <c r="F46">
+      <c r="F49">
         <v>-10</v>
       </c>
-      <c r="M46">
+      <c r="M49">
         <v>1300</v>
       </c>
-      <c r="N46" s="1">
+      <c r="N49" s="1">
         <f t="shared" si="1"/>
         <v>19.2</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>99</v>
-      </c>
-      <c r="B47" t="s">
-        <v>100</v>
-      </c>
-      <c r="C47">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>90</v>
+      </c>
+      <c r="B50" t="s">
+        <v>91</v>
+      </c>
+      <c r="C50">
         <v>12</v>
       </c>
-      <c r="D47">
+      <c r="D50">
         <v>0.27</v>
       </c>
-      <c r="E47">
+      <c r="E50">
         <v>-6</v>
       </c>
-      <c r="F47">
+      <c r="F50">
         <v>-13</v>
       </c>
-      <c r="M47">
+      <c r="M50">
         <v>1350</v>
       </c>
-      <c r="N47" s="1">
+      <c r="N50" s="1">
         <f t="shared" si="1"/>
         <v>19.2</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>101</v>
-      </c>
-      <c r="B48" t="s">
-        <v>102</v>
-      </c>
-      <c r="C48">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>92</v>
+      </c>
+      <c r="B51" t="s">
+        <v>93</v>
+      </c>
+      <c r="C51">
         <v>11</v>
       </c>
-      <c r="D48">
+      <c r="D51">
         <v>0.3</v>
       </c>
-      <c r="E48">
+      <c r="E51">
         <v>-7</v>
       </c>
-      <c r="F48">
+      <c r="F51">
         <v>-15</v>
       </c>
-      <c r="M48">
+      <c r="M51">
         <v>1400</v>
       </c>
-      <c r="N48" s="1">
+      <c r="N51" s="1">
         <f t="shared" si="1"/>
         <v>19.600000000000001</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>103</v>
-      </c>
-      <c r="B49" t="s">
-        <v>104</v>
-      </c>
-      <c r="C49">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>94</v>
+      </c>
+      <c r="B52" t="s">
+        <v>95</v>
+      </c>
+      <c r="C52">
         <v>9</v>
       </c>
-      <c r="D49">
+      <c r="D52">
         <v>0.34</v>
       </c>
-      <c r="E49">
+      <c r="E52">
         <v>-9</v>
       </c>
-      <c r="F49">
+      <c r="F52">
         <v>-17</v>
       </c>
-      <c r="M49">
+      <c r="M52">
         <v>1450</v>
       </c>
-      <c r="N49" s="1">
+      <c r="N52" s="1">
         <f t="shared" si="1"/>
         <v>19.599999999999998</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>105</v>
-      </c>
-      <c r="B50" t="s">
-        <v>106</v>
-      </c>
-      <c r="C50">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>96</v>
+      </c>
+      <c r="B53" t="s">
+        <v>97</v>
+      </c>
+      <c r="C53">
         <v>7</v>
       </c>
-      <c r="D50">
+      <c r="D53">
         <v>0.38</v>
       </c>
-      <c r="E50">
+      <c r="E53">
         <v>-11</v>
       </c>
-      <c r="F50">
+      <c r="F53">
         <v>-18</v>
       </c>
-      <c r="M50">
+      <c r="M53">
         <v>1500</v>
       </c>
-      <c r="N50" s="1">
+      <c r="N53" s="1">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>107</v>
-      </c>
-      <c r="B51" t="s">
-        <v>108</v>
-      </c>
-      <c r="C51">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>98</v>
+      </c>
+      <c r="B54" t="s">
+        <v>99</v>
+      </c>
+      <c r="C54">
         <v>5</v>
       </c>
-      <c r="D51">
+      <c r="D54">
         <v>0.42</v>
       </c>
-      <c r="E51">
+      <c r="E54">
         <v>-12</v>
       </c>
-      <c r="F51">
+      <c r="F54">
         <v>-20</v>
       </c>
-      <c r="M51">
+      <c r="M54">
         <v>1600</v>
       </c>
-      <c r="N51" s="1">
+      <c r="N54" s="1">
         <f t="shared" si="1"/>
         <v>18.200000000000003</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="N52" s="1">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N55" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>111</v>
-      </c>
-      <c r="B53" t="s">
-        <v>112</v>
-      </c>
-      <c r="C53">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>102</v>
+      </c>
+      <c r="B56" t="s">
+        <v>103</v>
+      </c>
+      <c r="C56">
         <v>-1</v>
       </c>
-      <c r="D53">
+      <c r="D56">
         <v>0.1</v>
       </c>
-      <c r="E53">
+      <c r="E56">
         <v>2</v>
       </c>
-      <c r="F53">
+      <c r="F56">
         <v>2</v>
       </c>
-      <c r="M53">
+      <c r="M56">
         <v>0</v>
       </c>
-      <c r="N53" s="1">
+      <c r="N56" s="1">
         <f t="shared" si="1"/>
         <v>-5.8</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>113</v>
-      </c>
-      <c r="B54" t="s">
-        <v>114</v>
-      </c>
-      <c r="C54">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>104</v>
+      </c>
+      <c r="B57" t="s">
+        <v>105</v>
+      </c>
+      <c r="C57">
         <v>-1</v>
       </c>
-      <c r="D54">
+      <c r="D57">
         <v>0.04</v>
       </c>
-      <c r="E54">
+      <c r="E57">
         <v>2</v>
       </c>
-      <c r="F54">
+      <c r="F57">
         <v>2</v>
       </c>
-      <c r="M54">
+      <c r="M57">
         <v>0</v>
       </c>
-      <c r="N54" s="1">
+      <c r="N57" s="1">
         <f t="shared" si="1"/>
         <v>-4.6000000000000005</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>115</v>
-      </c>
-      <c r="B55" t="s">
-        <v>112</v>
-      </c>
-      <c r="C55">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>106</v>
+      </c>
+      <c r="B58" t="s">
+        <v>103</v>
+      </c>
+      <c r="C58">
         <v>-1</v>
       </c>
-      <c r="D55">
+      <c r="D58">
         <v>0.1</v>
       </c>
-      <c r="M55">
+      <c r="M58">
         <v>0</v>
       </c>
-      <c r="N55" s="1">
+      <c r="N58" s="1">
         <f t="shared" si="1"/>
         <v>-3</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>116</v>
-      </c>
-      <c r="B56" t="s">
-        <v>114</v>
-      </c>
-      <c r="C56">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>107</v>
+      </c>
+      <c r="B59" t="s">
+        <v>105</v>
+      </c>
+      <c r="C59">
         <v>-1</v>
       </c>
-      <c r="D56">
+      <c r="D59">
         <v>0.04</v>
       </c>
-      <c r="M56">
+      <c r="M59">
         <v>0</v>
       </c>
-      <c r="N56" s="1">
+      <c r="N59" s="1">
         <f t="shared" si="1"/>
         <v>-1.8</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>117</v>
-      </c>
-      <c r="B57" t="s">
-        <v>112</v>
-      </c>
-      <c r="C57">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>108</v>
+      </c>
+      <c r="B60" t="s">
+        <v>103</v>
+      </c>
+      <c r="C60">
         <v>-1</v>
       </c>
-      <c r="D57">
+      <c r="D60">
         <v>0.1</v>
       </c>
-      <c r="M57">
+      <c r="M60">
         <v>0</v>
       </c>
-      <c r="N57" s="1">
+      <c r="N60" s="1">
         <f t="shared" si="1"/>
         <v>-3</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="N58" s="1">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N61" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>118</v>
-      </c>
-      <c r="B59" t="s">
-        <v>119</v>
-      </c>
-      <c r="C59">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>109</v>
+      </c>
+      <c r="B62" t="s">
+        <v>110</v>
+      </c>
+      <c r="C62">
         <v>-3</v>
       </c>
-      <c r="D59">
+      <c r="D62">
         <v>0.06</v>
       </c>
-      <c r="E59">
+      <c r="E62">
         <v>2</v>
       </c>
-      <c r="F59">
+      <c r="F62">
         <v>2</v>
       </c>
-      <c r="M59">
+      <c r="M62">
         <v>400</v>
       </c>
-      <c r="N59" s="1">
+      <c r="N62" s="1">
         <f t="shared" si="1"/>
         <v>-7.0000000000000009</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>120</v>
-      </c>
-      <c r="B60" t="s">
-        <v>121</v>
-      </c>
-      <c r="C60">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>111</v>
+      </c>
+      <c r="B63" t="s">
+        <v>112</v>
+      </c>
+      <c r="C63">
         <v>-2</v>
       </c>
-      <c r="D60">
+      <c r="D63">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="E60">
+      <c r="E63">
         <v>1</v>
       </c>
-      <c r="F60">
+      <c r="F63">
         <v>5</v>
       </c>
-      <c r="M60">
+      <c r="M63">
         <v>300</v>
       </c>
-      <c r="N60" s="1">
+      <c r="N63" s="1">
         <f t="shared" si="1"/>
         <v>-7.2</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>122</v>
-      </c>
-      <c r="B61" t="s">
-        <v>119</v>
-      </c>
-      <c r="C61">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>113</v>
+      </c>
+      <c r="B64" t="s">
+        <v>110</v>
+      </c>
+      <c r="C64">
         <v>-3</v>
       </c>
-      <c r="D61">
+      <c r="D64">
         <v>0.06</v>
       </c>
-      <c r="M61">
+      <c r="M64">
         <v>400</v>
       </c>
-      <c r="N61" s="1">
+      <c r="N64" s="1">
         <f t="shared" si="1"/>
         <v>-4.2</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>123</v>
-      </c>
-      <c r="B62" t="s">
-        <v>121</v>
-      </c>
-      <c r="C62">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>114</v>
+      </c>
+      <c r="B65" t="s">
+        <v>112</v>
+      </c>
+      <c r="C65">
         <v>-2</v>
       </c>
-      <c r="D62">
+      <c r="D65">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="M62">
+      <c r="M65">
         <v>300</v>
       </c>
-      <c r="N62" s="1">
+      <c r="N65" s="1">
         <f t="shared" si="1"/>
         <v>-3.4000000000000004</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N66" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>132</v>
+      </c>
+      <c r="B67" t="s">
+        <v>136</v>
+      </c>
+      <c r="C67">
+        <v>-2</v>
+      </c>
+      <c r="D67">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="M67">
+        <v>700</v>
+      </c>
+      <c r="N67" s="1">
+        <f t="shared" si="1"/>
+        <v>-3.4000000000000004</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>133</v>
+      </c>
+      <c r="B68" t="s">
+        <v>136</v>
+      </c>
+      <c r="C68">
+        <v>-2</v>
+      </c>
+      <c r="D68">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="M68">
+        <v>700</v>
+      </c>
+      <c r="N68" s="1">
+        <f t="shared" si="1"/>
+        <v>-3.4000000000000004</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>134</v>
+      </c>
+      <c r="B69" t="s">
+        <v>137</v>
+      </c>
+      <c r="C69">
+        <v>-1</v>
+      </c>
+      <c r="D69">
+        <v>0.04</v>
+      </c>
+      <c r="M69">
+        <v>300</v>
+      </c>
+      <c r="N69" s="1">
+        <f t="shared" si="1"/>
+        <v>-1.8</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>135</v>
+      </c>
+      <c r="B70" t="s">
+        <v>137</v>
+      </c>
+      <c r="C70">
+        <v>-1</v>
+      </c>
+      <c r="D70">
+        <v>0.04</v>
+      </c>
+      <c r="M70">
+        <v>300</v>
+      </c>
+      <c r="N70" s="1">
+        <f t="shared" si="1"/>
+        <v>-1.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>